<commit_message>
Add write k_kalibrate in ROM
</commit_message>
<xml_diff>
--- a/table_for_grafics.xlsx
+++ b/table_for_grafics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="38">
   <si>
     <t>Voltage</t>
   </si>
@@ -46,49 +46,40 @@
     <t>30</t>
   </si>
   <si>
+    <t>1.30</t>
+  </si>
+  <si>
+    <t>1.27</t>
+  </si>
+  <si>
+    <t>1.31</t>
+  </si>
+  <si>
     <t>1.29</t>
   </si>
   <si>
+    <t>1.32</t>
+  </si>
+  <si>
     <t>1.28</t>
   </si>
   <si>
     <t>1.33</t>
   </si>
   <si>
-    <t>1.27</t>
-  </si>
-  <si>
-    <t>0.00</t>
+    <t>1.37</t>
+  </si>
+  <si>
+    <t>1.26</t>
+  </si>
+  <si>
+    <t>1.41</t>
   </si>
   <si>
     <t>1.34</t>
   </si>
   <si>
-    <t>1.39</t>
-  </si>
-  <si>
-    <t>1.35</t>
-  </si>
-  <si>
-    <t>1.42</t>
-  </si>
-  <si>
-    <t>1.43</t>
-  </si>
-  <si>
-    <t>1.32</t>
-  </si>
-  <si>
-    <t>1.37</t>
-  </si>
-  <si>
-    <t>1.26</t>
-  </si>
-  <si>
-    <t>1.30</t>
-  </si>
-  <si>
-    <t>1.31</t>
+    <t>1.40</t>
   </si>
   <si>
     <t>1.14</t>
@@ -127,22 +118,16 @@
     <t>1.06</t>
   </si>
   <si>
+    <t>1.04</t>
+  </si>
+  <si>
     <t>1.07</t>
   </si>
   <si>
-    <t>1.04</t>
-  </si>
-  <si>
     <t>1.05</t>
   </si>
   <si>
     <t>1.03</t>
-  </si>
-  <si>
-    <t>51.22</t>
-  </si>
-  <si>
-    <t>14.58</t>
   </si>
 </sst>
 </file>
@@ -544,7 +529,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -555,7 +540,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -566,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -577,7 +562,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -588,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -599,7 +584,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -621,7 +606,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -632,7 +617,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -643,7 +628,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -654,7 +639,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -665,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -676,7 +661,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -687,7 +672,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -698,7 +683,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -709,7 +694,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -720,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -742,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -753,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -764,7 +749,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -775,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -786,7 +771,7 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -797,7 +782,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -808,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -819,7 +804,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -830,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -841,7 +826,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -852,7 +837,7 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -863,7 +848,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -874,7 +859,7 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -885,7 +870,7 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -896,7 +881,7 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -907,7 +892,7 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -918,7 +903,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -929,7 +914,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -940,7 +925,7 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -951,7 +936,7 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -962,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -973,7 +958,7 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -984,7 +969,7 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -995,7 +980,7 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1006,7 +991,7 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1017,7 +1002,7 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1028,7 +1013,7 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1039,7 +1024,7 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1050,7 +1035,7 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1061,7 +1046,7 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1072,7 +1057,7 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1083,7 +1068,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1094,7 +1079,7 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1105,7 +1090,7 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1127,7 +1112,7 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1138,7 +1123,7 @@
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1149,7 +1134,7 @@
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1160,7 +1145,7 @@
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1171,7 +1156,7 @@
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1193,7 +1178,7 @@
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1204,7 +1189,7 @@
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1215,7 +1200,7 @@
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1226,7 +1211,7 @@
         <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1237,7 +1222,7 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1248,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1259,7 +1244,7 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1270,7 +1255,7 @@
         <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1281,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1292,7 +1277,7 @@
         <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1303,7 +1288,7 @@
         <v>4</v>
       </c>
       <c r="C73" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1314,7 +1299,7 @@
         <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1325,7 +1310,7 @@
         <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1336,7 +1321,7 @@
         <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1347,7 +1332,7 @@
         <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1358,7 +1343,7 @@
         <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1369,7 +1354,7 @@
         <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1380,7 +1365,7 @@
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1391,7 +1376,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1402,7 +1387,7 @@
         <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1413,7 +1398,7 @@
         <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1424,7 +1409,7 @@
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1435,7 +1420,7 @@
         <v>4</v>
       </c>
       <c r="C85" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1446,7 +1431,7 @@
         <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1457,7 +1442,7 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1468,7 +1453,7 @@
         <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1479,7 +1464,7 @@
         <v>4</v>
       </c>
       <c r="C89" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1490,7 +1475,7 @@
         <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1501,7 +1486,7 @@
         <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1512,7 +1497,7 @@
         <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1523,7 +1508,7 @@
         <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1534,7 +1519,7 @@
         <v>4</v>
       </c>
       <c r="C94" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1545,7 +1530,7 @@
         <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1556,7 +1541,7 @@
         <v>4</v>
       </c>
       <c r="C96" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1567,7 +1552,7 @@
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1578,7 +1563,7 @@
         <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1589,7 +1574,7 @@
         <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1600,7 +1585,7 @@
         <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1611,7 +1596,7 @@
         <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1622,7 +1607,7 @@
         <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1633,7 +1618,7 @@
         <v>5</v>
       </c>
       <c r="C103" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1644,7 +1629,7 @@
         <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1655,7 +1640,7 @@
         <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -1666,7 +1651,7 @@
         <v>5</v>
       </c>
       <c r="C106" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1677,7 +1662,7 @@
         <v>5</v>
       </c>
       <c r="C107" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -1688,7 +1673,7 @@
         <v>5</v>
       </c>
       <c r="C108" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -1699,7 +1684,7 @@
         <v>5</v>
       </c>
       <c r="C109" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -1710,7 +1695,7 @@
         <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1721,7 +1706,7 @@
         <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -1732,7 +1717,7 @@
         <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -1743,7 +1728,7 @@
         <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -1754,7 +1739,7 @@
         <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -1765,7 +1750,7 @@
         <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1776,7 +1761,7 @@
         <v>5</v>
       </c>
       <c r="C116" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -1787,7 +1772,7 @@
         <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1798,7 +1783,7 @@
         <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -1809,7 +1794,7 @@
         <v>5</v>
       </c>
       <c r="C119" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1820,7 +1805,7 @@
         <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1831,7 +1816,7 @@
         <v>5</v>
       </c>
       <c r="C121" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1842,7 +1827,7 @@
         <v>5</v>
       </c>
       <c r="C122" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -1853,7 +1838,7 @@
         <v>5</v>
       </c>
       <c r="C123" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -1864,7 +1849,7 @@
         <v>5</v>
       </c>
       <c r="C124" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -1875,7 +1860,7 @@
         <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -1886,7 +1871,7 @@
         <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -1897,7 +1882,7 @@
         <v>5</v>
       </c>
       <c r="C127" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -1908,7 +1893,7 @@
         <v>5</v>
       </c>
       <c r="C128" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -1919,7 +1904,7 @@
         <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -1930,7 +1915,7 @@
         <v>6</v>
       </c>
       <c r="C130" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -1941,7 +1926,7 @@
         <v>6</v>
       </c>
       <c r="C131" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1952,7 +1937,7 @@
         <v>6</v>
       </c>
       <c r="C132" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -1963,7 +1948,7 @@
         <v>6</v>
       </c>
       <c r="C133" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -1974,7 +1959,7 @@
         <v>6</v>
       </c>
       <c r="C134" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1985,7 +1970,7 @@
         <v>6</v>
       </c>
       <c r="C135" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -1996,7 +1981,7 @@
         <v>6</v>
       </c>
       <c r="C136" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2007,7 +1992,7 @@
         <v>6</v>
       </c>
       <c r="C137" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2018,7 +2003,7 @@
         <v>6</v>
       </c>
       <c r="C138" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2029,7 +2014,7 @@
         <v>6</v>
       </c>
       <c r="C139" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2040,7 +2025,7 @@
         <v>6</v>
       </c>
       <c r="C140" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2051,7 +2036,7 @@
         <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2062,7 +2047,7 @@
         <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2073,7 +2058,7 @@
         <v>6</v>
       </c>
       <c r="C143" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2084,7 +2069,7 @@
         <v>6</v>
       </c>
       <c r="C144" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2095,7 +2080,7 @@
         <v>6</v>
       </c>
       <c r="C145" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2106,7 +2091,7 @@
         <v>6</v>
       </c>
       <c r="C146" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2117,7 +2102,7 @@
         <v>6</v>
       </c>
       <c r="C147" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2128,7 +2113,7 @@
         <v>6</v>
       </c>
       <c r="C148" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2139,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="C149" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2150,7 +2135,7 @@
         <v>6</v>
       </c>
       <c r="C150" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2161,7 +2146,7 @@
         <v>6</v>
       </c>
       <c r="C151" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2172,7 +2157,7 @@
         <v>6</v>
       </c>
       <c r="C152" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2183,7 +2168,7 @@
         <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2194,7 +2179,7 @@
         <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2205,7 +2190,7 @@
         <v>6</v>
       </c>
       <c r="C155" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2216,7 +2201,7 @@
         <v>6</v>
       </c>
       <c r="C156" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2227,7 +2212,7 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2238,7 +2223,7 @@
         <v>6</v>
       </c>
       <c r="C158" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2249,7 +2234,7 @@
         <v>6</v>
       </c>
       <c r="C159" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2260,7 +2245,7 @@
         <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2271,7 +2256,7 @@
         <v>6</v>
       </c>
       <c r="C161" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2282,7 +2267,7 @@
         <v>7</v>
       </c>
       <c r="C162" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2293,7 +2278,7 @@
         <v>7</v>
       </c>
       <c r="C163" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2304,7 +2289,7 @@
         <v>7</v>
       </c>
       <c r="C164" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2315,7 +2300,7 @@
         <v>7</v>
       </c>
       <c r="C165" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2326,7 +2311,7 @@
         <v>7</v>
       </c>
       <c r="C166" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2337,7 +2322,7 @@
         <v>7</v>
       </c>
       <c r="C167" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2359,7 +2344,7 @@
         <v>7</v>
       </c>
       <c r="C169" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2370,7 +2355,7 @@
         <v>7</v>
       </c>
       <c r="C170" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2381,7 +2366,7 @@
         <v>7</v>
       </c>
       <c r="C171" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2392,7 +2377,7 @@
         <v>7</v>
       </c>
       <c r="C172" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2403,7 +2388,7 @@
         <v>7</v>
       </c>
       <c r="C173" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2414,7 +2399,7 @@
         <v>7</v>
       </c>
       <c r="C174" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2425,7 +2410,7 @@
         <v>7</v>
       </c>
       <c r="C175" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2436,7 +2421,7 @@
         <v>7</v>
       </c>
       <c r="C176" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2447,7 +2432,7 @@
         <v>7</v>
       </c>
       <c r="C177" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2458,7 +2443,7 @@
         <v>7</v>
       </c>
       <c r="C178" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2469,7 +2454,7 @@
         <v>7</v>
       </c>
       <c r="C179" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2480,7 +2465,7 @@
         <v>7</v>
       </c>
       <c r="C180" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2491,7 +2476,7 @@
         <v>7</v>
       </c>
       <c r="C181" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2502,7 +2487,7 @@
         <v>7</v>
       </c>
       <c r="C182" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2513,7 +2498,7 @@
         <v>7</v>
       </c>
       <c r="C183" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -2524,7 +2509,7 @@
         <v>7</v>
       </c>
       <c r="C184" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -2535,7 +2520,7 @@
         <v>7</v>
       </c>
       <c r="C185" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -2546,7 +2531,7 @@
         <v>7</v>
       </c>
       <c r="C186" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -2557,7 +2542,7 @@
         <v>7</v>
       </c>
       <c r="C187" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -2568,7 +2553,7 @@
         <v>7</v>
       </c>
       <c r="C188" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -2579,7 +2564,7 @@
         <v>7</v>
       </c>
       <c r="C189" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -2590,7 +2575,7 @@
         <v>7</v>
       </c>
       <c r="C190" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -2612,7 +2597,7 @@
         <v>7</v>
       </c>
       <c r="C192" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -2623,7 +2608,7 @@
         <v>7</v>
       </c>
       <c r="C193" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -2634,7 +2619,7 @@
         <v>8</v>
       </c>
       <c r="C194" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -2645,7 +2630,7 @@
         <v>8</v>
       </c>
       <c r="C195" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -2656,7 +2641,7 @@
         <v>8</v>
       </c>
       <c r="C196" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -2667,7 +2652,7 @@
         <v>8</v>
       </c>
       <c r="C197" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -2678,7 +2663,7 @@
         <v>8</v>
       </c>
       <c r="C198" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -2689,7 +2674,7 @@
         <v>8</v>
       </c>
       <c r="C199" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -2700,7 +2685,7 @@
         <v>8</v>
       </c>
       <c r="C200" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -2711,7 +2696,7 @@
         <v>8</v>
       </c>
       <c r="C201" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -2722,7 +2707,7 @@
         <v>8</v>
       </c>
       <c r="C202" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -2733,7 +2718,7 @@
         <v>8</v>
       </c>
       <c r="C203" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -2744,7 +2729,7 @@
         <v>8</v>
       </c>
       <c r="C204" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -2755,7 +2740,7 @@
         <v>8</v>
       </c>
       <c r="C205" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -2766,7 +2751,7 @@
         <v>8</v>
       </c>
       <c r="C206" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -2777,7 +2762,7 @@
         <v>8</v>
       </c>
       <c r="C207" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -2788,7 +2773,7 @@
         <v>8</v>
       </c>
       <c r="C208" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -2799,7 +2784,7 @@
         <v>8</v>
       </c>
       <c r="C209" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -2810,7 +2795,7 @@
         <v>8</v>
       </c>
       <c r="C210" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -2821,7 +2806,7 @@
         <v>8</v>
       </c>
       <c r="C211" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -2832,7 +2817,7 @@
         <v>8</v>
       </c>
       <c r="C212" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -2843,7 +2828,7 @@
         <v>8</v>
       </c>
       <c r="C213" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -2854,7 +2839,7 @@
         <v>8</v>
       </c>
       <c r="C214" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -2865,7 +2850,7 @@
         <v>8</v>
       </c>
       <c r="C215" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -2876,7 +2861,7 @@
         <v>8</v>
       </c>
       <c r="C216" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -2887,7 +2872,7 @@
         <v>8</v>
       </c>
       <c r="C217" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -2898,7 +2883,7 @@
         <v>8</v>
       </c>
       <c r="C218" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -2909,7 +2894,7 @@
         <v>8</v>
       </c>
       <c r="C219" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -2920,7 +2905,7 @@
         <v>8</v>
       </c>
       <c r="C220" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -2931,7 +2916,7 @@
         <v>8</v>
       </c>
       <c r="C221" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -2942,7 +2927,7 @@
         <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -2953,7 +2938,7 @@
         <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -2964,7 +2949,7 @@
         <v>8</v>
       </c>
       <c r="C224" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -2975,7 +2960,7 @@
         <v>8</v>
       </c>
       <c r="C225" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -2986,7 +2971,7 @@
         <v>9</v>
       </c>
       <c r="C226" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -2997,7 +2982,7 @@
         <v>9</v>
       </c>
       <c r="C227" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3008,7 +2993,7 @@
         <v>9</v>
       </c>
       <c r="C228" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3019,7 +3004,7 @@
         <v>9</v>
       </c>
       <c r="C229" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3030,7 +3015,7 @@
         <v>9</v>
       </c>
       <c r="C230" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3041,7 +3026,7 @@
         <v>9</v>
       </c>
       <c r="C231" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3052,7 +3037,7 @@
         <v>9</v>
       </c>
       <c r="C232" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3063,7 +3048,7 @@
         <v>9</v>
       </c>
       <c r="C233" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3074,7 +3059,7 @@
         <v>9</v>
       </c>
       <c r="C234" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3085,7 +3070,7 @@
         <v>9</v>
       </c>
       <c r="C235" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3096,7 +3081,7 @@
         <v>9</v>
       </c>
       <c r="C236" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3107,7 +3092,7 @@
         <v>9</v>
       </c>
       <c r="C237" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3118,7 +3103,7 @@
         <v>9</v>
       </c>
       <c r="C238" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3129,7 +3114,7 @@
         <v>9</v>
       </c>
       <c r="C239" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3140,7 +3125,7 @@
         <v>9</v>
       </c>
       <c r="C240" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3151,7 +3136,7 @@
         <v>9</v>
       </c>
       <c r="C241" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3162,7 +3147,7 @@
         <v>9</v>
       </c>
       <c r="C242" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3173,7 +3158,7 @@
         <v>9</v>
       </c>
       <c r="C243" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3184,7 +3169,7 @@
         <v>9</v>
       </c>
       <c r="C244" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3195,7 +3180,7 @@
         <v>9</v>
       </c>
       <c r="C245" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3206,7 +3191,7 @@
         <v>9</v>
       </c>
       <c r="C246" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3217,7 +3202,7 @@
         <v>9</v>
       </c>
       <c r="C247" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3228,7 +3213,7 @@
         <v>9</v>
       </c>
       <c r="C248" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3239,7 +3224,7 @@
         <v>9</v>
       </c>
       <c r="C249" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3250,7 +3235,7 @@
         <v>9</v>
       </c>
       <c r="C250" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3261,7 +3246,7 @@
         <v>9</v>
       </c>
       <c r="C251" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3272,7 +3257,7 @@
         <v>9</v>
       </c>
       <c r="C252" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3283,7 +3268,7 @@
         <v>9</v>
       </c>
       <c r="C253" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -3294,7 +3279,7 @@
         <v>9</v>
       </c>
       <c r="C254" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -3305,7 +3290,7 @@
         <v>9</v>
       </c>
       <c r="C255" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -3316,7 +3301,7 @@
         <v>9</v>
       </c>
       <c r="C256" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -3327,7 +3312,7 @@
         <v>9</v>
       </c>
       <c r="C257" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add write K_polinoms in ROM
</commit_message>
<xml_diff>
--- a/table_for_grafics.xlsx
+++ b/table_for_grafics.xlsx
@@ -46,22 +46,34 @@
     <t>30</t>
   </si>
   <si>
+    <t>1.31</t>
+  </si>
+  <si>
+    <t>1.28</t>
+  </si>
+  <si>
+    <t>1.29</t>
+  </si>
+  <si>
     <t>1.30</t>
   </si>
   <si>
-    <t>1.27</t>
-  </si>
-  <si>
-    <t>1.31</t>
-  </si>
-  <si>
-    <t>1.29</t>
-  </si>
-  <si>
     <t>1.32</t>
   </si>
   <si>
-    <t>1.28</t>
+    <t>1.36</t>
+  </si>
+  <si>
+    <t>1.40</t>
+  </si>
+  <si>
+    <t>1.34</t>
+  </si>
+  <si>
+    <t>1.42</t>
+  </si>
+  <si>
+    <t>1.26</t>
   </si>
   <si>
     <t>1.33</t>
@@ -70,18 +82,6 @@
     <t>1.37</t>
   </si>
   <si>
-    <t>1.26</t>
-  </si>
-  <si>
-    <t>1.41</t>
-  </si>
-  <si>
-    <t>1.34</t>
-  </si>
-  <si>
-    <t>1.40</t>
-  </si>
-  <si>
     <t>1.14</t>
   </si>
   <si>
@@ -91,15 +91,15 @@
     <t>1.13</t>
   </si>
   <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>1.16</t>
+  </si>
+  <si>
     <t>1.15</t>
   </si>
   <si>
-    <t>1.16</t>
-  </si>
-  <si>
-    <t>1.11</t>
-  </si>
-  <si>
     <t>1.17</t>
   </si>
   <si>
@@ -115,13 +115,13 @@
     <t>1.09</t>
   </si>
   <si>
+    <t>1.07</t>
+  </si>
+  <si>
     <t>1.06</t>
   </si>
   <si>
     <t>1.04</t>
-  </si>
-  <si>
-    <t>1.07</t>
   </si>
   <si>
     <t>1.05</t>
@@ -562,7 +562,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -573,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -584,7 +584,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -595,7 +595,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -606,7 +606,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -617,7 +617,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -639,7 +639,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -650,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -661,7 +661,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -672,7 +672,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -683,7 +683,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -694,7 +694,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -705,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -716,7 +716,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -727,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -738,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -771,7 +771,7 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -782,7 +782,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -793,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -804,7 +804,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -815,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -826,7 +826,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -837,7 +837,7 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -848,7 +848,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -903,7 +903,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -914,7 +914,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -925,7 +925,7 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -947,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -991,7 +991,7 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1002,7 +1002,7 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1024,7 +1024,7 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1046,7 +1046,7 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1079,7 +1079,7 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1101,7 +1101,7 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1112,7 +1112,7 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1156,7 +1156,7 @@
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1167,7 +1167,7 @@
         <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1244,7 +1244,7 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1343,7 +1343,7 @@
         <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1354,7 +1354,7 @@
         <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1376,7 +1376,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1398,7 +1398,7 @@
         <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1442,7 +1442,7 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1453,7 +1453,7 @@
         <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1464,7 +1464,7 @@
         <v>4</v>
       </c>
       <c r="C89" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1508,7 +1508,7 @@
         <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1519,7 +1519,7 @@
         <v>4</v>
       </c>
       <c r="C94" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1541,7 +1541,7 @@
         <v>4</v>
       </c>
       <c r="C96" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1574,7 +1574,7 @@
         <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1585,7 +1585,7 @@
         <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1618,7 +1618,7 @@
         <v>5</v>
       </c>
       <c r="C103" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1695,7 +1695,7 @@
         <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1772,7 +1772,7 @@
         <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1783,7 +1783,7 @@
         <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -1805,7 +1805,7 @@
         <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1838,7 +1838,7 @@
         <v>5</v>
       </c>
       <c r="C123" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -1871,7 +1871,7 @@
         <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -1904,7 +1904,7 @@
         <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -1915,7 +1915,7 @@
         <v>6</v>
       </c>
       <c r="C130" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -1926,7 +1926,7 @@
         <v>6</v>
       </c>
       <c r="C131" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1937,7 +1937,7 @@
         <v>6</v>
       </c>
       <c r="C132" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -1948,7 +1948,7 @@
         <v>6</v>
       </c>
       <c r="C133" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -1959,7 +1959,7 @@
         <v>6</v>
       </c>
       <c r="C134" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1970,7 +1970,7 @@
         <v>6</v>
       </c>
       <c r="C135" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -1981,7 +1981,7 @@
         <v>6</v>
       </c>
       <c r="C136" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -1992,7 +1992,7 @@
         <v>6</v>
       </c>
       <c r="C137" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2003,7 +2003,7 @@
         <v>6</v>
       </c>
       <c r="C138" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2025,7 +2025,7 @@
         <v>6</v>
       </c>
       <c r="C140" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2036,7 +2036,7 @@
         <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2047,7 +2047,7 @@
         <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2058,7 +2058,7 @@
         <v>6</v>
       </c>
       <c r="C143" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2069,7 +2069,7 @@
         <v>6</v>
       </c>
       <c r="C144" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2080,7 +2080,7 @@
         <v>6</v>
       </c>
       <c r="C145" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2091,7 +2091,7 @@
         <v>6</v>
       </c>
       <c r="C146" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2102,7 +2102,7 @@
         <v>6</v>
       </c>
       <c r="C147" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2113,7 +2113,7 @@
         <v>6</v>
       </c>
       <c r="C148" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2124,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="C149" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2135,7 +2135,7 @@
         <v>6</v>
       </c>
       <c r="C150" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2146,7 +2146,7 @@
         <v>6</v>
       </c>
       <c r="C151" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2157,7 +2157,7 @@
         <v>6</v>
       </c>
       <c r="C152" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2168,7 +2168,7 @@
         <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2179,7 +2179,7 @@
         <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2190,7 +2190,7 @@
         <v>6</v>
       </c>
       <c r="C155" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2212,7 +2212,7 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2223,7 +2223,7 @@
         <v>6</v>
       </c>
       <c r="C158" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2234,7 +2234,7 @@
         <v>6</v>
       </c>
       <c r="C159" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2245,7 +2245,7 @@
         <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2256,7 +2256,7 @@
         <v>6</v>
       </c>
       <c r="C161" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2267,7 +2267,7 @@
         <v>7</v>
       </c>
       <c r="C162" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2278,7 +2278,7 @@
         <v>7</v>
       </c>
       <c r="C163" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2311,7 +2311,7 @@
         <v>7</v>
       </c>
       <c r="C166" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2322,7 +2322,7 @@
         <v>7</v>
       </c>
       <c r="C167" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2344,7 +2344,7 @@
         <v>7</v>
       </c>
       <c r="C169" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2355,7 +2355,7 @@
         <v>7</v>
       </c>
       <c r="C170" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2366,7 +2366,7 @@
         <v>7</v>
       </c>
       <c r="C171" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2388,7 +2388,7 @@
         <v>7</v>
       </c>
       <c r="C173" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2399,7 +2399,7 @@
         <v>7</v>
       </c>
       <c r="C174" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2410,7 +2410,7 @@
         <v>7</v>
       </c>
       <c r="C175" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2421,7 +2421,7 @@
         <v>7</v>
       </c>
       <c r="C176" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2432,7 +2432,7 @@
         <v>7</v>
       </c>
       <c r="C177" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2454,7 +2454,7 @@
         <v>7</v>
       </c>
       <c r="C179" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2465,7 +2465,7 @@
         <v>7</v>
       </c>
       <c r="C180" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2476,7 +2476,7 @@
         <v>7</v>
       </c>
       <c r="C181" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2498,7 +2498,7 @@
         <v>7</v>
       </c>
       <c r="C183" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -2509,7 +2509,7 @@
         <v>7</v>
       </c>
       <c r="C184" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -2520,7 +2520,7 @@
         <v>7</v>
       </c>
       <c r="C185" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -2531,7 +2531,7 @@
         <v>7</v>
       </c>
       <c r="C186" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -2553,7 +2553,7 @@
         <v>7</v>
       </c>
       <c r="C188" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -2564,7 +2564,7 @@
         <v>7</v>
       </c>
       <c r="C189" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -2575,7 +2575,7 @@
         <v>7</v>
       </c>
       <c r="C190" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -2586,7 +2586,7 @@
         <v>7</v>
       </c>
       <c r="C191" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -2718,7 +2718,7 @@
         <v>8</v>
       </c>
       <c r="C203" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -2762,7 +2762,7 @@
         <v>8</v>
       </c>
       <c r="C207" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -2773,7 +2773,7 @@
         <v>8</v>
       </c>
       <c r="C208" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -2784,7 +2784,7 @@
         <v>8</v>
       </c>
       <c r="C209" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -2806,7 +2806,7 @@
         <v>8</v>
       </c>
       <c r="C211" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -2817,7 +2817,7 @@
         <v>8</v>
       </c>
       <c r="C212" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -2828,7 +2828,7 @@
         <v>8</v>
       </c>
       <c r="C213" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -2861,7 +2861,7 @@
         <v>8</v>
       </c>
       <c r="C216" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -2872,7 +2872,7 @@
         <v>8</v>
       </c>
       <c r="C217" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -2916,7 +2916,7 @@
         <v>8</v>
       </c>
       <c r="C221" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -3070,7 +3070,7 @@
         <v>9</v>
       </c>
       <c r="C235" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3114,7 +3114,7 @@
         <v>9</v>
       </c>
       <c r="C239" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3125,7 +3125,7 @@
         <v>9</v>
       </c>
       <c r="C240" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3136,7 +3136,7 @@
         <v>9</v>
       </c>
       <c r="C241" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3158,7 +3158,7 @@
         <v>9</v>
       </c>
       <c r="C243" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3169,7 +3169,7 @@
         <v>9</v>
       </c>
       <c r="C244" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3180,7 +3180,7 @@
         <v>9</v>
       </c>
       <c r="C245" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3202,7 +3202,7 @@
         <v>9</v>
       </c>
       <c r="C247" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3268,7 +3268,7 @@
         <v>9</v>
       </c>
       <c r="C253" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="254" spans="1:3">

</xml_diff>

<commit_message>
NEW calibrate and Stage 03
</commit_message>
<xml_diff>
--- a/table_for_grafics.xlsx
+++ b/table_for_grafics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="37">
   <si>
     <t>Voltage</t>
   </si>
@@ -46,88 +46,85 @@
     <t>30</t>
   </si>
   <si>
+    <t>1.57</t>
+  </si>
+  <si>
+    <t>1.63</t>
+  </si>
+  <si>
+    <t>1.54</t>
+  </si>
+  <si>
+    <t>1.60</t>
+  </si>
+  <si>
+    <t>1.51</t>
+  </si>
+  <si>
+    <t>1.70</t>
+  </si>
+  <si>
+    <t>1.40</t>
+  </si>
+  <si>
+    <t>1.39</t>
+  </si>
+  <si>
+    <t>1.37</t>
+  </si>
+  <si>
+    <t>1.43</t>
+  </si>
+  <si>
+    <t>1.41</t>
+  </si>
+  <si>
+    <t>1.38</t>
+  </si>
+  <si>
+    <t>1.35</t>
+  </si>
+  <si>
+    <t>1.46</t>
+  </si>
+  <si>
+    <t>1.47</t>
+  </si>
+  <si>
+    <t>1.48</t>
+  </si>
+  <si>
+    <t>1.45</t>
+  </si>
+  <si>
+    <t>1.33</t>
+  </si>
+  <si>
+    <t>1.36</t>
+  </si>
+  <si>
+    <t>1.34</t>
+  </si>
+  <si>
     <t>1.31</t>
   </si>
   <si>
+    <t>1.42</t>
+  </si>
+  <si>
+    <t>1.32</t>
+  </si>
+  <si>
+    <t>1.29</t>
+  </si>
+  <si>
+    <t>1.30</t>
+  </si>
+  <si>
     <t>1.28</t>
   </si>
   <si>
-    <t>1.29</t>
-  </si>
-  <si>
-    <t>1.30</t>
-  </si>
-  <si>
-    <t>1.32</t>
-  </si>
-  <si>
-    <t>1.36</t>
-  </si>
-  <si>
-    <t>1.40</t>
-  </si>
-  <si>
-    <t>1.34</t>
-  </si>
-  <si>
-    <t>1.42</t>
-  </si>
-  <si>
-    <t>1.26</t>
-  </si>
-  <si>
-    <t>1.33</t>
-  </si>
-  <si>
-    <t>1.37</t>
-  </si>
-  <si>
-    <t>1.14</t>
-  </si>
-  <si>
-    <t>1.12</t>
-  </si>
-  <si>
-    <t>1.13</t>
-  </si>
-  <si>
-    <t>1.11</t>
-  </si>
-  <si>
-    <t>1.16</t>
-  </si>
-  <si>
-    <t>1.15</t>
-  </si>
-  <si>
-    <t>1.17</t>
-  </si>
-  <si>
-    <t>1.18</t>
-  </si>
-  <si>
-    <t>1.10</t>
-  </si>
-  <si>
-    <t>1.08</t>
-  </si>
-  <si>
-    <t>1.09</t>
-  </si>
-  <si>
-    <t>1.07</t>
-  </si>
-  <si>
-    <t>1.06</t>
-  </si>
-  <si>
-    <t>1.04</t>
-  </si>
-  <si>
-    <t>1.05</t>
-  </si>
-  <si>
-    <t>1.03</t>
+    <t>2.00</t>
   </si>
 </sst>
 </file>
@@ -518,7 +515,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -529,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -540,7 +537,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -551,7 +548,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -562,7 +559,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -573,7 +570,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -584,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -595,7 +592,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -606,7 +603,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -617,7 +614,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -628,7 +625,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -639,7 +636,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -650,7 +647,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -661,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -672,7 +669,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -683,7 +680,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -694,7 +691,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -705,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -716,7 +713,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -727,7 +724,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -738,7 +735,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -749,7 +746,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -760,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -771,7 +768,7 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -782,7 +779,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -793,7 +790,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -804,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -815,7 +812,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -826,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -848,7 +845,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -859,7 +856,7 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -870,7 +867,7 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -881,7 +878,7 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -892,7 +889,7 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -903,7 +900,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -914,7 +911,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -925,7 +922,7 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -936,7 +933,7 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -947,7 +944,7 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -958,7 +955,7 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -969,7 +966,7 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -980,7 +977,7 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -991,7 +988,7 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1002,7 +999,7 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1013,7 +1010,7 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1024,7 +1021,7 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1035,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1046,7 +1043,7 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1057,7 +1054,7 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1068,7 +1065,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1079,7 +1076,7 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1090,7 +1087,7 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1101,7 +1098,7 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1112,7 +1109,7 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1123,7 +1120,7 @@
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1134,7 +1131,7 @@
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1145,7 +1142,7 @@
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1156,7 +1153,7 @@
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1167,7 +1164,7 @@
         <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1178,7 +1175,7 @@
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1189,7 +1186,7 @@
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1200,7 +1197,7 @@
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1211,7 +1208,7 @@
         <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1222,7 +1219,7 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1233,7 +1230,7 @@
         <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1244,7 +1241,7 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1255,7 +1252,7 @@
         <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1266,7 +1263,7 @@
         <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1277,7 +1274,7 @@
         <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1288,7 +1285,7 @@
         <v>4</v>
       </c>
       <c r="C73" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1299,7 +1296,7 @@
         <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1310,7 +1307,7 @@
         <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1321,7 +1318,7 @@
         <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1332,7 +1329,7 @@
         <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1343,7 +1340,7 @@
         <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1354,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1365,7 +1362,7 @@
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1376,7 +1373,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1387,7 +1384,7 @@
         <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1398,7 +1395,7 @@
         <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1409,7 +1406,7 @@
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1420,7 +1417,7 @@
         <v>4</v>
       </c>
       <c r="C85" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1431,7 +1428,7 @@
         <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1442,7 +1439,7 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1453,7 +1450,7 @@
         <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1464,7 +1461,7 @@
         <v>4</v>
       </c>
       <c r="C89" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1475,7 +1472,7 @@
         <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1486,7 +1483,7 @@
         <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1497,7 +1494,7 @@
         <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1508,7 +1505,7 @@
         <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1519,7 +1516,7 @@
         <v>4</v>
       </c>
       <c r="C94" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1530,7 +1527,7 @@
         <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1541,7 +1538,7 @@
         <v>4</v>
       </c>
       <c r="C96" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1552,7 +1549,7 @@
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1563,7 +1560,7 @@
         <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1574,7 +1571,7 @@
         <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1585,7 +1582,7 @@
         <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1596,7 +1593,7 @@
         <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1607,7 +1604,7 @@
         <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1618,7 +1615,7 @@
         <v>5</v>
       </c>
       <c r="C103" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1629,7 +1626,7 @@
         <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1640,7 +1637,7 @@
         <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -1651,7 +1648,7 @@
         <v>5</v>
       </c>
       <c r="C106" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1662,7 +1659,7 @@
         <v>5</v>
       </c>
       <c r="C107" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -1673,7 +1670,7 @@
         <v>5</v>
       </c>
       <c r="C108" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -1684,7 +1681,7 @@
         <v>5</v>
       </c>
       <c r="C109" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -1695,7 +1692,7 @@
         <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1706,7 +1703,7 @@
         <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -1717,7 +1714,7 @@
         <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -1728,7 +1725,7 @@
         <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -1739,7 +1736,7 @@
         <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -1750,7 +1747,7 @@
         <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1761,7 +1758,7 @@
         <v>5</v>
       </c>
       <c r="C116" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -1772,7 +1769,7 @@
         <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1783,7 +1780,7 @@
         <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -1794,7 +1791,7 @@
         <v>5</v>
       </c>
       <c r="C119" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1805,7 +1802,7 @@
         <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1816,7 +1813,7 @@
         <v>5</v>
       </c>
       <c r="C121" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1827,7 +1824,7 @@
         <v>5</v>
       </c>
       <c r="C122" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -1838,7 +1835,7 @@
         <v>5</v>
       </c>
       <c r="C123" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -1849,7 +1846,7 @@
         <v>5</v>
       </c>
       <c r="C124" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -1860,7 +1857,7 @@
         <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -1871,7 +1868,7 @@
         <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -1882,7 +1879,7 @@
         <v>5</v>
       </c>
       <c r="C127" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -1893,7 +1890,7 @@
         <v>5</v>
       </c>
       <c r="C128" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -1904,7 +1901,7 @@
         <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -1915,7 +1912,7 @@
         <v>6</v>
       </c>
       <c r="C130" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -1926,7 +1923,7 @@
         <v>6</v>
       </c>
       <c r="C131" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1937,7 +1934,7 @@
         <v>6</v>
       </c>
       <c r="C132" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -1948,7 +1945,7 @@
         <v>6</v>
       </c>
       <c r="C133" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -1959,7 +1956,7 @@
         <v>6</v>
       </c>
       <c r="C134" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1970,7 +1967,7 @@
         <v>6</v>
       </c>
       <c r="C135" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -1992,7 +1989,7 @@
         <v>6</v>
       </c>
       <c r="C137" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2003,7 +2000,7 @@
         <v>6</v>
       </c>
       <c r="C138" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2014,7 +2011,7 @@
         <v>6</v>
       </c>
       <c r="C139" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2025,7 +2022,7 @@
         <v>6</v>
       </c>
       <c r="C140" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2036,7 +2033,7 @@
         <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2058,7 +2055,7 @@
         <v>6</v>
       </c>
       <c r="C143" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2069,7 +2066,7 @@
         <v>6</v>
       </c>
       <c r="C144" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2080,7 +2077,7 @@
         <v>6</v>
       </c>
       <c r="C145" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2091,7 +2088,7 @@
         <v>6</v>
       </c>
       <c r="C146" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2102,7 +2099,7 @@
         <v>6</v>
       </c>
       <c r="C147" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2113,7 +2110,7 @@
         <v>6</v>
       </c>
       <c r="C148" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2124,7 +2121,7 @@
         <v>6</v>
       </c>
       <c r="C149" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2135,7 +2132,7 @@
         <v>6</v>
       </c>
       <c r="C150" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2146,7 +2143,7 @@
         <v>6</v>
       </c>
       <c r="C151" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2157,7 +2154,7 @@
         <v>6</v>
       </c>
       <c r="C152" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2168,7 +2165,7 @@
         <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2179,7 +2176,7 @@
         <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2190,7 +2187,7 @@
         <v>6</v>
       </c>
       <c r="C155" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2201,7 +2198,7 @@
         <v>6</v>
       </c>
       <c r="C156" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2212,7 +2209,7 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2223,7 +2220,7 @@
         <v>6</v>
       </c>
       <c r="C158" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2234,7 +2231,7 @@
         <v>6</v>
       </c>
       <c r="C159" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2245,7 +2242,7 @@
         <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2256,7 +2253,7 @@
         <v>6</v>
       </c>
       <c r="C161" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2267,7 +2264,7 @@
         <v>7</v>
       </c>
       <c r="C162" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2278,7 +2275,7 @@
         <v>7</v>
       </c>
       <c r="C163" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2289,7 +2286,7 @@
         <v>7</v>
       </c>
       <c r="C164" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2300,7 +2297,7 @@
         <v>7</v>
       </c>
       <c r="C165" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2311,7 +2308,7 @@
         <v>7</v>
       </c>
       <c r="C166" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2322,7 +2319,7 @@
         <v>7</v>
       </c>
       <c r="C167" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2333,7 +2330,7 @@
         <v>7</v>
       </c>
       <c r="C168" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2344,7 +2341,7 @@
         <v>7</v>
       </c>
       <c r="C169" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2355,7 +2352,7 @@
         <v>7</v>
       </c>
       <c r="C170" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2366,7 +2363,7 @@
         <v>7</v>
       </c>
       <c r="C171" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2377,7 +2374,7 @@
         <v>7</v>
       </c>
       <c r="C172" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2388,7 +2385,7 @@
         <v>7</v>
       </c>
       <c r="C173" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2399,7 +2396,7 @@
         <v>7</v>
       </c>
       <c r="C174" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2410,7 +2407,7 @@
         <v>7</v>
       </c>
       <c r="C175" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2421,7 +2418,7 @@
         <v>7</v>
       </c>
       <c r="C176" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2432,7 +2429,7 @@
         <v>7</v>
       </c>
       <c r="C177" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2443,7 +2440,7 @@
         <v>7</v>
       </c>
       <c r="C178" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2454,7 +2451,7 @@
         <v>7</v>
       </c>
       <c r="C179" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2465,7 +2462,7 @@
         <v>7</v>
       </c>
       <c r="C180" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2476,7 +2473,7 @@
         <v>7</v>
       </c>
       <c r="C181" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2487,7 +2484,7 @@
         <v>7</v>
       </c>
       <c r="C182" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2498,7 +2495,7 @@
         <v>7</v>
       </c>
       <c r="C183" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -2509,7 +2506,7 @@
         <v>7</v>
       </c>
       <c r="C184" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -2520,7 +2517,7 @@
         <v>7</v>
       </c>
       <c r="C185" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -2531,7 +2528,7 @@
         <v>7</v>
       </c>
       <c r="C186" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -2542,7 +2539,7 @@
         <v>7</v>
       </c>
       <c r="C187" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -2553,7 +2550,7 @@
         <v>7</v>
       </c>
       <c r="C188" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -2564,7 +2561,7 @@
         <v>7</v>
       </c>
       <c r="C189" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -2575,7 +2572,7 @@
         <v>7</v>
       </c>
       <c r="C190" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -2586,7 +2583,7 @@
         <v>7</v>
       </c>
       <c r="C191" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -2597,7 +2594,7 @@
         <v>7</v>
       </c>
       <c r="C192" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -2608,7 +2605,7 @@
         <v>7</v>
       </c>
       <c r="C193" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -2619,7 +2616,7 @@
         <v>8</v>
       </c>
       <c r="C194" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -2630,7 +2627,7 @@
         <v>8</v>
       </c>
       <c r="C195" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -2641,7 +2638,7 @@
         <v>8</v>
       </c>
       <c r="C196" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -2652,7 +2649,7 @@
         <v>8</v>
       </c>
       <c r="C197" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -2663,7 +2660,7 @@
         <v>8</v>
       </c>
       <c r="C198" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -2674,7 +2671,7 @@
         <v>8</v>
       </c>
       <c r="C199" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -2685,7 +2682,7 @@
         <v>8</v>
       </c>
       <c r="C200" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -2696,7 +2693,7 @@
         <v>8</v>
       </c>
       <c r="C201" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -2707,7 +2704,7 @@
         <v>8</v>
       </c>
       <c r="C202" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -2718,7 +2715,7 @@
         <v>8</v>
       </c>
       <c r="C203" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -2729,7 +2726,7 @@
         <v>8</v>
       </c>
       <c r="C204" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -2740,7 +2737,7 @@
         <v>8</v>
       </c>
       <c r="C205" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -2751,7 +2748,7 @@
         <v>8</v>
       </c>
       <c r="C206" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -2762,7 +2759,7 @@
         <v>8</v>
       </c>
       <c r="C207" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -2773,7 +2770,7 @@
         <v>8</v>
       </c>
       <c r="C208" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -2784,7 +2781,7 @@
         <v>8</v>
       </c>
       <c r="C209" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -2795,7 +2792,7 @@
         <v>8</v>
       </c>
       <c r="C210" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -2806,7 +2803,7 @@
         <v>8</v>
       </c>
       <c r="C211" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -2817,7 +2814,7 @@
         <v>8</v>
       </c>
       <c r="C212" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -2828,7 +2825,7 @@
         <v>8</v>
       </c>
       <c r="C213" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -2839,7 +2836,7 @@
         <v>8</v>
       </c>
       <c r="C214" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -2850,7 +2847,7 @@
         <v>8</v>
       </c>
       <c r="C215" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -2861,7 +2858,7 @@
         <v>8</v>
       </c>
       <c r="C216" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -2872,7 +2869,7 @@
         <v>8</v>
       </c>
       <c r="C217" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -2883,7 +2880,7 @@
         <v>8</v>
       </c>
       <c r="C218" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -2894,7 +2891,7 @@
         <v>8</v>
       </c>
       <c r="C219" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -2905,7 +2902,7 @@
         <v>8</v>
       </c>
       <c r="C220" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -2916,7 +2913,7 @@
         <v>8</v>
       </c>
       <c r="C221" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -2927,7 +2924,7 @@
         <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -2938,7 +2935,7 @@
         <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -2949,7 +2946,7 @@
         <v>8</v>
       </c>
       <c r="C224" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -2960,7 +2957,7 @@
         <v>8</v>
       </c>
       <c r="C225" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -2971,7 +2968,7 @@
         <v>9</v>
       </c>
       <c r="C226" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -2982,7 +2979,7 @@
         <v>9</v>
       </c>
       <c r="C227" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -2993,7 +2990,7 @@
         <v>9</v>
       </c>
       <c r="C228" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3004,7 +3001,7 @@
         <v>9</v>
       </c>
       <c r="C229" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3015,7 +3012,7 @@
         <v>9</v>
       </c>
       <c r="C230" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3026,7 +3023,7 @@
         <v>9</v>
       </c>
       <c r="C231" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3037,7 +3034,7 @@
         <v>9</v>
       </c>
       <c r="C232" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3048,7 +3045,7 @@
         <v>9</v>
       </c>
       <c r="C233" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3059,7 +3056,7 @@
         <v>9</v>
       </c>
       <c r="C234" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3070,7 +3067,7 @@
         <v>9</v>
       </c>
       <c r="C235" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3081,7 +3078,7 @@
         <v>9</v>
       </c>
       <c r="C236" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3092,7 +3089,7 @@
         <v>9</v>
       </c>
       <c r="C237" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3103,7 +3100,7 @@
         <v>9</v>
       </c>
       <c r="C238" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3114,7 +3111,7 @@
         <v>9</v>
       </c>
       <c r="C239" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3125,7 +3122,7 @@
         <v>9</v>
       </c>
       <c r="C240" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3136,7 +3133,7 @@
         <v>9</v>
       </c>
       <c r="C241" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3147,7 +3144,7 @@
         <v>9</v>
       </c>
       <c r="C242" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3158,7 +3155,7 @@
         <v>9</v>
       </c>
       <c r="C243" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3169,7 +3166,7 @@
         <v>9</v>
       </c>
       <c r="C244" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3180,7 +3177,7 @@
         <v>9</v>
       </c>
       <c r="C245" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3191,7 +3188,7 @@
         <v>9</v>
       </c>
       <c r="C246" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3202,7 +3199,7 @@
         <v>9</v>
       </c>
       <c r="C247" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3213,7 +3210,7 @@
         <v>9</v>
       </c>
       <c r="C248" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3224,7 +3221,7 @@
         <v>9</v>
       </c>
       <c r="C249" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3235,7 +3232,7 @@
         <v>9</v>
       </c>
       <c r="C250" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3246,7 +3243,7 @@
         <v>9</v>
       </c>
       <c r="C251" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3257,7 +3254,7 @@
         <v>9</v>
       </c>
       <c r="C252" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3268,7 +3265,7 @@
         <v>9</v>
       </c>
       <c r="C253" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -3279,7 +3276,7 @@
         <v>9</v>
       </c>
       <c r="C254" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -3290,7 +3287,7 @@
         <v>9</v>
       </c>
       <c r="C255" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -3301,7 +3298,7 @@
         <v>9</v>
       </c>
       <c r="C256" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -3312,7 +3309,7 @@
         <v>9</v>
       </c>
       <c r="C257" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>